<commit_message>
Updated excel documents to read ANep as well as removed any data sets that did not include pT > 1.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1000.xlsx
+++ b/database/AN_ep/expdata/1000.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malda\Documents\GitHub\jam3d\database\AN_ep\expdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C7A14-778A-4473-8268-1A9D695FD465}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5406" yWindow="0" windowWidth="9870" windowHeight="8172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -55,14 +61,14 @@
     <t>HERMES</t>
   </si>
   <si>
-    <t>AN</t>
+    <t>ANep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -171,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,6 +269,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,14 +462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,21 +503,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>0.0718</v>
+        <v>7.1800000000000003E-2</v>
       </c>
       <c r="B2">
-        <v>1.1002</v>
+        <v>1.1002000000000001</v>
       </c>
       <c r="C2">
-        <v>0.0162</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="D2">
-        <v>0.0119</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>0.0057</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="F2">
         <v>7.25</v>
@@ -483,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0.1045</v>
       </c>
@@ -491,13 +543,13 @@
         <v>1.1173</v>
       </c>
       <c r="C3">
-        <v>0.013</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>0.0064</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="E3">
-        <v>0.0036</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="F3">
         <v>7.25</v>
@@ -515,21 +567,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>0.1383</v>
+        <v>0.13830000000000001</v>
       </c>
       <c r="B4">
-        <v>1.132</v>
+        <v>1.1319999999999999</v>
       </c>
       <c r="C4">
-        <v>0.0162</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="D4">
-        <v>0.0051</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="E4">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="F4">
         <v>7.25</v>
@@ -547,21 +599,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0.1729</v>
       </c>
       <c r="B5">
-        <v>1.1396</v>
+        <v>1.1395999999999999</v>
       </c>
       <c r="C5">
-        <v>0.0022</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>0.0051</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="E5">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F5">
         <v>7.25</v>
@@ -579,21 +631,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>0.2075</v>
+        <v>0.20749999999999999</v>
       </c>
       <c r="B6">
-        <v>1.1465</v>
+        <v>1.1465000000000001</v>
       </c>
       <c r="C6">
-        <v>-0.0011</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="D6">
-        <v>0.0055</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="E6">
-        <v>0.0046</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="F6">
         <v>7.25</v>
@@ -611,21 +663,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>0.242</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="B7">
         <v>1.1616</v>
       </c>
       <c r="C7">
-        <v>0.0005999999999999999</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="D7">
-        <v>0.0061</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="E7">
-        <v>0.0049</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="F7">
         <v>7.25</v>
@@ -643,21 +695,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>0.2793</v>
+        <v>0.27929999999999999</v>
       </c>
       <c r="B8">
         <v>1.1811</v>
       </c>
       <c r="C8">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D8">
-        <v>0.0065</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="E8">
-        <v>0.0047</v>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="F8">
         <v>7.25</v>
@@ -675,21 +727,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>0.3188</v>
+        <v>0.31879999999999997</v>
       </c>
       <c r="B9">
-        <v>1.1962</v>
+        <v>1.1961999999999999</v>
       </c>
       <c r="C9">
-        <v>-0.0024</v>
+        <v>-2.3999999999999998E-3</v>
       </c>
       <c r="D9">
-        <v>0.0075</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E9">
-        <v>0.0068</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="F9">
         <v>7.25</v>
@@ -707,21 +759,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>0.3588</v>
+        <v>0.35880000000000001</v>
       </c>
       <c r="B10">
         <v>1.2119</v>
       </c>
       <c r="C10">
-        <v>-0.0049</v>
+        <v>-4.8999999999999998E-3</v>
       </c>
       <c r="D10">
-        <v>0.0086</v>
+        <v>8.6E-3</v>
       </c>
       <c r="E10">
-        <v>0.007900000000000001</v>
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="F10">
         <v>7.25</v>
@@ -739,21 +791,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>0.3988</v>
+        <v>0.39879999999999999</v>
       </c>
       <c r="B11">
-        <v>1.2092</v>
+        <v>1.2092000000000001</v>
       </c>
       <c r="C11">
-        <v>0.0057</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="D11">
-        <v>0.0098</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="E11">
-        <v>0.0081</v>
+        <v>8.0999999999999996E-3</v>
       </c>
       <c r="F11">
         <v>7.25</v>
@@ -771,21 +823,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <v>0.446</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="B12">
         <v>1.1652</v>
       </c>
       <c r="C12">
-        <v>-0.0228</v>
+        <v>-2.2800000000000001E-2</v>
       </c>
       <c r="D12">
         <v>0.01</v>
       </c>
       <c r="E12">
-        <v>0.009299999999999999</v>
+        <v>9.2999999999999992E-3</v>
       </c>
       <c r="F12">
         <v>7.25</v>
@@ -803,21 +855,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <v>0.4866</v>
+        <v>0.48659999999999998</v>
       </c>
       <c r="B13">
         <v>1.0622</v>
       </c>
       <c r="C13">
-        <v>-0.0509</v>
+        <v>-5.0900000000000001E-2</v>
       </c>
       <c r="D13">
-        <v>0.0333</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="E13">
-        <v>0.0252</v>
+        <v>2.52E-2</v>
       </c>
       <c r="F13">
         <v>7.25</v>

</xml_diff>